<commit_message>
Ajouts en cours menus pesées
</commit_message>
<xml_diff>
--- a/jauges.xlsx
+++ b/jauges.xlsx
@@ -377,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +418,7 @@
         <v>254556</v>
       </c>
       <c r="I2">
-        <f>G2/poids</f>
+        <f t="shared" ref="I2:I10" si="0">G2/poids</f>
         <v>109204.63320463321</v>
       </c>
     </row>
@@ -433,11 +433,11 @@
         <v>227141</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G5" si="0">+E3-C3</f>
+        <f t="shared" ref="G3:G4" si="1">+E3-C3</f>
         <v>248782</v>
       </c>
       <c r="I3">
-        <f>G3/poids</f>
+        <f t="shared" si="0"/>
         <v>106727.58472758473</v>
       </c>
     </row>
@@ -452,11 +452,11 @@
         <v>361627</v>
       </c>
       <c r="G4">
+        <f t="shared" si="1"/>
+        <v>240760</v>
+      </c>
+      <c r="I4">
         <f t="shared" si="0"/>
-        <v>240760</v>
-      </c>
-      <c r="I4">
-        <f>G4/poids</f>
         <v>103286.14328614328</v>
       </c>
     </row>
@@ -475,17 +475,17 @@
         <v>243290</v>
       </c>
       <c r="I5">
-        <f>G5/poids</f>
+        <f t="shared" si="0"/>
         <v>104371.51437151438</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G6">
-        <f t="shared" ref="G6:G8" si="1">+E6-C6</f>
+        <f t="shared" ref="G6:G8" si="2">+E6-C6</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>G6/poids</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -500,11 +500,11 @@
         <v>-75900</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-54100</v>
       </c>
       <c r="I7">
-        <f>G7/poids</f>
+        <f t="shared" si="0"/>
         <v>-23208.92320892321</v>
       </c>
     </row>
@@ -519,11 +519,11 @@
         <v>-88863</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-53112</v>
       </c>
       <c r="I8">
-        <f>G8/poids</f>
+        <f t="shared" si="0"/>
         <v>-22785.070785070784</v>
       </c>
     </row>
@@ -538,17 +538,34 @@
         <v>-81617</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9" si="2">+E9-C9</f>
+        <f t="shared" ref="G9:G10" si="3">+E9-C9</f>
         <v>-53591</v>
       </c>
       <c r="I9">
-        <f>G9/poids</f>
+        <f t="shared" si="0"/>
         <v>-22990.56199056199</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-142358</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-362886</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>-220528</v>
+      </c>
+      <c r="H10">
+        <v>11000</v>
+      </c>
+      <c r="I10">
+        <f>G10/11</f>
+        <v>-20048</v>
       </c>
       <c r="J10" t="s">
         <v>7</v>

</xml_diff>